<commit_message>
updated a mistake on the burndown chart
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 2/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint 2/Burndown chart.xlsx
@@ -670,8 +670,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="403290403"/>
-        <c:axId val="1185948852"/>
+        <c:axId val="803707489"/>
+        <c:axId val="167531753"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -745,11 +745,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="403290403"/>
-        <c:axId val="1185948852"/>
+        <c:axId val="803707489"/>
+        <c:axId val="167531753"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="403290403"/>
+        <c:axId val="803707489"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,10 +801,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1185948852"/>
+        <c:crossAx val="167531753"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1185948852"/>
+        <c:axId val="167531753"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="22.0"/>
@@ -869,7 +869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="403290403"/>
+        <c:crossAx val="803707489"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1356,24 +1356,24 @@
         <v>6</v>
       </c>
       <c r="E13" s="43">
-        <f>$D$13-($D$13/15*1)</f>
-        <v>5.6</v>
+        <f>$D$13-($D$13/5*1)</f>
+        <v>4.8</v>
       </c>
       <c r="F13" s="44">
-        <f>$D$13-($D$13/15*2)</f>
-        <v>5.2</v>
+        <f>$D$13-($D$13/5*2)</f>
+        <v>3.6</v>
       </c>
       <c r="G13" s="44">
-        <f>$D$13-($D$13/15*3)</f>
-        <v>4.8</v>
+        <f>$D$13-($D$13/5*3)</f>
+        <v>2.4</v>
       </c>
       <c r="H13" s="44">
-        <f>$D$13-($D$13/15*4)</f>
-        <v>4.4</v>
+        <f>$D$13-($D$13/5*4)</f>
+        <v>1.2</v>
       </c>
       <c r="I13" s="44">
-        <f>$D$13-($D$13/15*5)</f>
-        <v>4</v>
+        <f>$D$13-($D$13/5*5)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1"/>

</xml_diff>